<commit_message>
Various changes and VAE implementation
</commit_message>
<xml_diff>
--- a/ocean/notebooks/metrics.xlsx
+++ b/ocean/notebooks/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,26 @@
           <t>Average SSIM between Model Output and HR</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Average EK between LR and HR</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Average EK between Model Output and HR</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Average Acc between LR and HR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Average Acc between Model Output and HR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -473,6 +493,18 @@
       <c r="E2" t="n">
         <v>0.9837353536093959</v>
       </c>
+      <c r="F2" t="n">
+        <v>8.522042723894119</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.53161281367143</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9627068261299901</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.9948936274063523</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -492,6 +524,18 @@
       <c r="E3" t="n">
         <v>0.9130922782536705</v>
       </c>
+      <c r="F3" t="n">
+        <v>20.49433722813924</v>
+      </c>
+      <c r="G3" t="n">
+        <v>11.80521180232366</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.7566254261269123</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.9395661467287658</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -511,6 +555,18 @@
       <c r="E4" t="n">
         <v>0.8079061388233308</v>
       </c>
+      <c r="F4" t="n">
+        <v>32.23843422253927</v>
+      </c>
+      <c r="G4" t="n">
+        <v>23.81968121210734</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4969428583524946</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7006880093674811</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -530,6 +586,18 @@
       <c r="E5" t="n">
         <v>0.9838476719406075</v>
       </c>
+      <c r="F5" t="n">
+        <v>8.559897836446762</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.493587876955668</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.961297985508244</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9949249328997131</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -549,6 +617,18 @@
       <c r="E6" t="n">
         <v>0.9162036504327982</v>
       </c>
+      <c r="F6" t="n">
+        <v>20.58161719322204</v>
+      </c>
+      <c r="G6" t="n">
+        <v>11.85936235427856</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.7489690695827318</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.9372976741223997</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -567,6 +647,18 @@
       </c>
       <c r="E7" t="n">
         <v>0.811492004088801</v>
+      </c>
+      <c r="F7" t="n">
+        <v>32.14891414324443</v>
+      </c>
+      <c r="G7" t="n">
+        <v>23.48789763450623</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.4872306777600225</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7050356599753942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>